<commit_message>
fix problem in the split childrens
</commit_message>
<xml_diff>
--- a/Projects/NESTLEUK_SAND/Data/Nestle_UK_v3.0.xlsx
+++ b/Projects/NESTLEUK_SAND/Data/Nestle_UK_v3.0.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="KPIs" sheetId="1" state="visible" r:id="rId2"/>
@@ -139,7 +139,7 @@
     <t>Confectionery Singles FTG - Superstores</t>
   </si>
   <si>
-    <t>Impulse - Confectionery FTG</t>
+    <t>Impulse - Confectionery Food to Go</t>
   </si>
   <si>
     <t>GR1 - Superstores FTG</t>
@@ -603,7 +603,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="67">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -694,6 +694,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -948,26 +952,26 @@
   </sheetPr>
   <dimension ref="A1:M51"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="E45" activeCellId="0" sqref="E45"/>
+      <selection pane="bottomLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="34.8137651821862"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="31.5991902834008"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.8866396761134"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="30.6356275303644"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.3522267206478"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="21.1012145748988"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="15.5303643724696"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="21.7449392712551"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="32.0283400809717"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="35.2429149797571"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="32.0283400809717"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="33.4210526315789"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="31.17004048583"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.5668016194332"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="21.3157894736842"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="15.7449392712551"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="22.1740890688259"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="32.4574898785425"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="0" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="0" width="11.0323886639676"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="10.1781376518219"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="14" min="14" style="0" width="5.89068825910931"/>
     <col collapsed="false" hidden="false" max="15" min="15" style="0" width="11.6761133603239"/>
     <col collapsed="false" hidden="false" max="1025" min="16" style="0" width="8.57085020242915"/>
@@ -1343,7 +1347,7 @@
       <c r="L12" s="20"/>
       <c r="M12" s="22"/>
     </row>
-    <row r="13" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="6" t="s">
         <v>37</v>
       </c>
@@ -1351,7 +1355,7 @@
       <c r="C13" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D13" s="7" t="s">
+      <c r="D13" s="23" t="s">
         <v>38</v>
       </c>
       <c r="E13" s="6" t="s">
@@ -1370,7 +1374,7 @@
       </c>
       <c r="M13" s="13"/>
     </row>
-    <row r="14" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="10" t="s">
         <v>39</v>
       </c>
@@ -1380,7 +1384,7 @@
       <c r="C14" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D14" s="7" t="s">
+      <c r="D14" s="23" t="s">
         <v>38</v>
       </c>
       <c r="E14" s="6" t="s">
@@ -1401,7 +1405,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="10" t="s">
         <v>40</v>
       </c>
@@ -1411,7 +1415,7 @@
       <c r="C15" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D15" s="7" t="s">
+      <c r="D15" s="23" t="s">
         <v>38</v>
       </c>
       <c r="E15" s="6" t="s">
@@ -1432,7 +1436,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="10" t="s">
         <v>41</v>
       </c>
@@ -1442,7 +1446,7 @@
       <c r="C16" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D16" s="7" t="s">
+      <c r="D16" s="23" t="s">
         <v>38</v>
       </c>
       <c r="E16" s="6" t="s">
@@ -1463,7 +1467,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="10" t="s">
         <v>22</v>
       </c>
@@ -1473,7 +1477,7 @@
       <c r="C17" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D17" s="7" t="s">
+      <c r="D17" s="23" t="s">
         <v>38</v>
       </c>
       <c r="E17" s="8"/>
@@ -1494,7 +1498,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="12" t="s">
         <v>26</v>
       </c>
@@ -1504,7 +1508,7 @@
       <c r="C18" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D18" s="7" t="s">
+      <c r="D18" s="23" t="s">
         <v>38</v>
       </c>
       <c r="E18" s="8"/>
@@ -1521,7 +1525,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="12" t="s">
         <v>29</v>
       </c>
@@ -1531,7 +1535,7 @@
       <c r="C19" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D19" s="7" t="s">
+      <c r="D19" s="23" t="s">
         <v>38</v>
       </c>
       <c r="E19" s="8"/>
@@ -1548,7 +1552,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="12" t="s">
         <v>31</v>
       </c>
@@ -1558,7 +1562,7 @@
       <c r="C20" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D20" s="7" t="s">
+      <c r="D20" s="23" t="s">
         <v>38</v>
       </c>
       <c r="E20" s="8"/>
@@ -1579,7 +1583,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="12" t="s">
         <v>34</v>
       </c>
@@ -1589,7 +1593,7 @@
       <c r="C21" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D21" s="7" t="s">
+      <c r="D21" s="23" t="s">
         <v>38</v>
       </c>
       <c r="E21" s="8"/>
@@ -1610,7 +1614,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="8" t="s">
         <v>36</v>
       </c>
@@ -1620,7 +1624,7 @@
       <c r="C22" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D22" s="7" t="s">
+      <c r="D22" s="23" t="s">
         <v>38</v>
       </c>
       <c r="E22" s="8"/>
@@ -1857,7 +1861,7 @@
       <c r="L30" s="20"/>
       <c r="M30" s="22"/>
     </row>
-    <row r="31" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="8" t="s">
         <v>47</v>
       </c>
@@ -1865,7 +1869,7 @@
       <c r="C31" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="D31" s="7" t="s">
+      <c r="D31" s="23" t="s">
         <v>38</v>
       </c>
       <c r="E31" s="8" t="s">
@@ -1884,7 +1888,7 @@
       </c>
       <c r="M31" s="13"/>
     </row>
-    <row r="32" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="8" t="s">
         <v>48</v>
       </c>
@@ -1894,7 +1898,7 @@
       <c r="C32" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="D32" s="7" t="s">
+      <c r="D32" s="23" t="s">
         <v>38</v>
       </c>
       <c r="E32" s="8" t="s">
@@ -1915,7 +1919,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="8" t="s">
         <v>22</v>
       </c>
@@ -1925,7 +1929,7 @@
       <c r="C33" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="D33" s="7" t="s">
+      <c r="D33" s="23" t="s">
         <v>38</v>
       </c>
       <c r="E33" s="8" t="s">
@@ -1948,7 +1952,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="8" t="s">
         <v>26</v>
       </c>
@@ -1958,7 +1962,7 @@
       <c r="C34" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="D34" s="7" t="s">
+      <c r="D34" s="23" t="s">
         <v>38</v>
       </c>
       <c r="E34" s="8" t="s">
@@ -1979,7 +1983,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="8" t="s">
         <v>29</v>
       </c>
@@ -1989,7 +1993,7 @@
       <c r="C35" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="D35" s="7" t="s">
+      <c r="D35" s="23" t="s">
         <v>38</v>
       </c>
       <c r="E35" s="8" t="s">
@@ -2010,7 +2014,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="8" t="s">
         <v>31</v>
       </c>
@@ -2020,7 +2024,7 @@
       <c r="C36" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="D36" s="7" t="s">
+      <c r="D36" s="23" t="s">
         <v>38</v>
       </c>
       <c r="E36" s="8" t="s">
@@ -2303,7 +2307,7 @@
       </c>
     </row>
     <row r="46" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="23" t="s">
+      <c r="A46" s="24" t="s">
         <v>61</v>
       </c>
       <c r="B46" s="8" t="s">
@@ -2322,12 +2326,12 @@
       <c r="G46" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="H46" s="24"/>
-      <c r="I46" s="24" t="s">
+      <c r="H46" s="25"/>
+      <c r="I46" s="25" t="s">
         <v>62</v>
       </c>
-      <c r="J46" s="24"/>
-      <c r="K46" s="25"/>
+      <c r="J46" s="25"/>
+      <c r="K46" s="26"/>
       <c r="L46" s="8" t="s">
         <v>25</v>
       </c>
@@ -2336,7 +2340,7 @@
       </c>
     </row>
     <row r="47" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="23" t="s">
+      <c r="A47" s="24" t="s">
         <v>63</v>
       </c>
       <c r="B47" s="8" t="s">
@@ -2355,12 +2359,12 @@
       <c r="G47" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="H47" s="24"/>
-      <c r="I47" s="24" t="s">
+      <c r="H47" s="25"/>
+      <c r="I47" s="25" t="s">
         <v>64</v>
       </c>
-      <c r="J47" s="24"/>
-      <c r="K47" s="25"/>
+      <c r="J47" s="25"/>
+      <c r="K47" s="26"/>
       <c r="L47" s="8" t="s">
         <v>25</v>
       </c>
@@ -2369,7 +2373,7 @@
       </c>
     </row>
     <row r="48" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="23" t="s">
+      <c r="A48" s="24" t="s">
         <v>65</v>
       </c>
       <c r="B48" s="8" t="s">
@@ -2388,12 +2392,12 @@
       <c r="G48" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="H48" s="24"/>
-      <c r="I48" s="24" t="s">
+      <c r="H48" s="25"/>
+      <c r="I48" s="25" t="s">
         <v>66</v>
       </c>
-      <c r="J48" s="24"/>
-      <c r="K48" s="25"/>
+      <c r="J48" s="25"/>
+      <c r="K48" s="26"/>
       <c r="L48" s="8" t="s">
         <v>25</v>
       </c>
@@ -2402,7 +2406,7 @@
       </c>
     </row>
     <row r="49" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="23" t="s">
+      <c r="A49" s="24" t="s">
         <v>67</v>
       </c>
       <c r="B49" s="8" t="s">
@@ -2419,14 +2423,14 @@
       </c>
       <c r="F49" s="8"/>
       <c r="G49" s="8"/>
-      <c r="H49" s="24" t="s">
+      <c r="H49" s="25" t="s">
         <v>69</v>
       </c>
-      <c r="I49" s="24" t="s">
+      <c r="I49" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="J49" s="24"/>
-      <c r="K49" s="25" t="n">
+      <c r="J49" s="25"/>
+      <c r="K49" s="26" t="n">
         <v>0.4</v>
       </c>
       <c r="L49" s="8" t="s">
@@ -2437,7 +2441,7 @@
       </c>
     </row>
     <row r="50" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="26" t="s">
+      <c r="A50" s="27" t="s">
         <v>70</v>
       </c>
       <c r="B50" s="8" t="s">
@@ -2460,8 +2464,8 @@
       <c r="I50" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="J50" s="24"/>
-      <c r="K50" s="25" t="n">
+      <c r="J50" s="25"/>
+      <c r="K50" s="26" t="n">
         <v>0.25</v>
       </c>
       <c r="L50" s="8" t="s">
@@ -2472,19 +2476,19 @@
       </c>
     </row>
     <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="27"/>
-      <c r="B51" s="28"/>
-      <c r="C51" s="28"/>
-      <c r="D51" s="29"/>
-      <c r="E51" s="30"/>
-      <c r="F51" s="30"/>
-      <c r="G51" s="30"/>
-      <c r="H51" s="30"/>
-      <c r="I51" s="30"/>
-      <c r="J51" s="31"/>
-      <c r="K51" s="32"/>
-      <c r="L51" s="33"/>
-      <c r="M51" s="34"/>
+      <c r="A51" s="28"/>
+      <c r="B51" s="29"/>
+      <c r="C51" s="29"/>
+      <c r="D51" s="30"/>
+      <c r="E51" s="31"/>
+      <c r="F51" s="31"/>
+      <c r="G51" s="31"/>
+      <c r="H51" s="31"/>
+      <c r="I51" s="31"/>
+      <c r="J51" s="32"/>
+      <c r="K51" s="33"/>
+      <c r="L51" s="34"/>
+      <c r="M51" s="35"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -2504,285 +2508,285 @@
   </sheetPr>
   <dimension ref="B2:J65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G26" activeCellId="0" sqref="G26"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H12" activeCellId="0" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.3198380566802"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="40.5991902834008"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.4939271255061"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="38.0283400809717"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="24.5303643724696"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="24.3157894736842"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="24.5303643724696"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="25.2793522267206"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.5303643724696"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="41.2388663967611"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.7085020242915"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="38.668016194332"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="24.9595141700405"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="24.7449392712551"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="24.9595141700405"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="25.6032388663968"/>
     <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="3" customFormat="false" ht="19.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G3" s="35" t="s">
+      <c r="G3" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="H3" s="35"/>
-      <c r="I3" s="35"/>
-      <c r="J3" s="35"/>
+      <c r="H3" s="36"/>
+      <c r="I3" s="36"/>
+      <c r="J3" s="36"/>
     </row>
     <row r="4" customFormat="false" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G4" s="36" t="s">
-        <v>14</v>
-      </c>
-      <c r="H4" s="36"/>
-      <c r="I4" s="36" t="s">
+      <c r="G4" s="37" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" s="37"/>
+      <c r="I4" s="37" t="s">
         <v>44</v>
       </c>
-      <c r="J4" s="36"/>
-    </row>
-    <row r="5" customFormat="false" ht="16.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="37" t="s">
+      <c r="J4" s="37"/>
+    </row>
+    <row r="5" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="37" t="s">
+      <c r="C5" s="38" t="s">
         <v>71</v>
       </c>
-      <c r="D5" s="37" t="s">
+      <c r="D5" s="38" t="s">
         <v>72</v>
       </c>
-      <c r="E5" s="37" t="s">
+      <c r="E5" s="38" t="s">
         <v>73</v>
       </c>
-      <c r="F5" s="37" t="s">
+      <c r="F5" s="38" t="s">
         <v>74</v>
       </c>
-      <c r="G5" s="38" t="s">
+      <c r="G5" s="39" t="s">
         <v>15</v>
       </c>
-      <c r="H5" s="39" t="s">
+      <c r="H5" s="40" t="s">
         <v>38</v>
       </c>
-      <c r="I5" s="38" t="s">
+      <c r="I5" s="39" t="s">
         <v>15</v>
       </c>
-      <c r="J5" s="39" t="s">
+      <c r="J5" s="40" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="40" t="s">
+      <c r="B6" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="41" t="s">
+      <c r="C6" s="42" t="s">
         <v>75</v>
       </c>
-      <c r="D6" s="42"/>
-      <c r="E6" s="43" t="s">
+      <c r="D6" s="43"/>
+      <c r="E6" s="44" t="s">
         <v>75</v>
       </c>
-      <c r="F6" s="44" t="n">
+      <c r="F6" s="45" t="n">
         <v>7613035220065</v>
       </c>
-      <c r="G6" s="45" t="n">
-        <v>1</v>
-      </c>
-      <c r="H6" s="46" t="n">
-        <v>1</v>
-      </c>
-      <c r="I6" s="45" t="n">
-        <v>1</v>
-      </c>
-      <c r="J6" s="46" t="n">
+      <c r="G6" s="46" t="n">
+        <v>1</v>
+      </c>
+      <c r="H6" s="47" t="n">
+        <v>1</v>
+      </c>
+      <c r="I6" s="46" t="n">
+        <v>1</v>
+      </c>
+      <c r="J6" s="47" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="47" t="s">
+      <c r="B7" s="48" t="s">
         <v>22</v>
       </c>
       <c r="C7" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="D7" s="48"/>
-      <c r="E7" s="49" t="s">
+      <c r="D7" s="49"/>
+      <c r="E7" s="50" t="s">
         <v>76</v>
       </c>
-      <c r="F7" s="50" t="n">
+      <c r="F7" s="51" t="n">
         <v>7613034954459</v>
       </c>
-      <c r="G7" s="51" t="n">
-        <v>1</v>
-      </c>
-      <c r="H7" s="52" t="n">
-        <v>1</v>
-      </c>
-      <c r="I7" s="51" t="n">
-        <v>1</v>
-      </c>
-      <c r="J7" s="52" t="n">
+      <c r="G7" s="52" t="n">
+        <v>1</v>
+      </c>
+      <c r="H7" s="53" t="n">
+        <v>1</v>
+      </c>
+      <c r="I7" s="52" t="n">
+        <v>1</v>
+      </c>
+      <c r="J7" s="53" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="47" t="s">
+      <c r="B8" s="48" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="53" t="s">
+      <c r="C8" s="54" t="s">
         <v>77</v>
       </c>
-      <c r="D8" s="54"/>
-      <c r="E8" s="55" t="s">
+      <c r="D8" s="55"/>
+      <c r="E8" s="56" t="s">
         <v>77</v>
       </c>
-      <c r="F8" s="56" t="n">
+      <c r="F8" s="57" t="n">
         <v>7613035058347</v>
       </c>
-      <c r="G8" s="51" t="n">
-        <v>1</v>
-      </c>
-      <c r="H8" s="52" t="n">
-        <v>1</v>
-      </c>
-      <c r="I8" s="51" t="n">
-        <v>1</v>
-      </c>
-      <c r="J8" s="52" t="n">
+      <c r="G8" s="52" t="n">
+        <v>1</v>
+      </c>
+      <c r="H8" s="53" t="n">
+        <v>1</v>
+      </c>
+      <c r="I8" s="52" t="n">
+        <v>1</v>
+      </c>
+      <c r="J8" s="53" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="47" t="s">
+      <c r="B9" s="48" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="53" t="s">
+      <c r="C9" s="54" t="s">
         <v>78</v>
       </c>
-      <c r="D9" s="54"/>
-      <c r="E9" s="55" t="s">
+      <c r="D9" s="55"/>
+      <c r="E9" s="56" t="s">
         <v>78</v>
       </c>
-      <c r="F9" s="56" t="n">
+      <c r="F9" s="57" t="n">
         <v>7613034872630</v>
       </c>
-      <c r="G9" s="51" t="n">
-        <v>1</v>
-      </c>
-      <c r="H9" s="52" t="n">
-        <v>1</v>
-      </c>
-      <c r="I9" s="51" t="n">
-        <v>1</v>
-      </c>
-      <c r="J9" s="52" t="n">
+      <c r="G9" s="52" t="n">
+        <v>1</v>
+      </c>
+      <c r="H9" s="53" t="n">
+        <v>1</v>
+      </c>
+      <c r="I9" s="52" t="n">
+        <v>1</v>
+      </c>
+      <c r="J9" s="53" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="47" t="s">
+      <c r="B10" s="48" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="53" t="s">
+      <c r="C10" s="54" t="s">
         <v>79</v>
       </c>
-      <c r="D10" s="54"/>
-      <c r="E10" s="55" t="s">
+      <c r="D10" s="55"/>
+      <c r="E10" s="56" t="s">
         <v>79</v>
       </c>
-      <c r="F10" s="56" t="n">
+      <c r="F10" s="57" t="n">
         <v>50251414</v>
       </c>
-      <c r="G10" s="51" t="n">
-        <v>1</v>
-      </c>
-      <c r="H10" s="52" t="n">
-        <v>1</v>
-      </c>
-      <c r="I10" s="51" t="n">
-        <v>1</v>
-      </c>
-      <c r="J10" s="52" t="n">
+      <c r="G10" s="52" t="n">
+        <v>1</v>
+      </c>
+      <c r="H10" s="53" t="n">
+        <v>1</v>
+      </c>
+      <c r="I10" s="52" t="n">
+        <v>1</v>
+      </c>
+      <c r="J10" s="53" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="47" t="s">
+      <c r="B11" s="48" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="53" t="s">
+      <c r="C11" s="54" t="s">
         <v>80</v>
       </c>
-      <c r="D11" s="54"/>
-      <c r="E11" s="55" t="s">
+      <c r="D11" s="55"/>
+      <c r="E11" s="56" t="s">
         <v>80</v>
       </c>
-      <c r="F11" s="56" t="n">
+      <c r="F11" s="57" t="n">
         <v>50189779</v>
       </c>
-      <c r="G11" s="51" t="n">
-        <v>1</v>
-      </c>
-      <c r="H11" s="52" t="n">
-        <v>1</v>
-      </c>
-      <c r="I11" s="51" t="n">
-        <v>1</v>
-      </c>
-      <c r="J11" s="52" t="n">
+      <c r="G11" s="52" t="n">
+        <v>1</v>
+      </c>
+      <c r="H11" s="53" t="n">
+        <v>1</v>
+      </c>
+      <c r="I11" s="52" t="n">
+        <v>1</v>
+      </c>
+      <c r="J11" s="53" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="47" t="s">
+      <c r="B12" s="48" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="53" t="s">
+      <c r="C12" s="54" t="s">
         <v>81</v>
       </c>
-      <c r="D12" s="54"/>
-      <c r="E12" s="55" t="s">
+      <c r="D12" s="55"/>
+      <c r="E12" s="56" t="s">
         <v>81</v>
       </c>
-      <c r="F12" s="56" t="n">
+      <c r="F12" s="57" t="n">
         <v>7613035738119</v>
       </c>
-      <c r="G12" s="51" t="n">
-        <v>1</v>
-      </c>
-      <c r="H12" s="52" t="n">
-        <v>1</v>
-      </c>
-      <c r="I12" s="51" t="n">
-        <v>1</v>
-      </c>
-      <c r="J12" s="52" t="n">
+      <c r="G12" s="52" t="n">
+        <v>1</v>
+      </c>
+      <c r="H12" s="53" t="n">
+        <v>1</v>
+      </c>
+      <c r="I12" s="52" t="n">
+        <v>1</v>
+      </c>
+      <c r="J12" s="53" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="30.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="57" t="s">
+      <c r="B13" s="58" t="s">
         <v>22</v>
       </c>
-      <c r="C13" s="58" t="s">
+      <c r="C13" s="59" t="s">
         <v>82</v>
       </c>
-      <c r="D13" s="59"/>
-      <c r="E13" s="60" t="s">
+      <c r="D13" s="60"/>
+      <c r="E13" s="61" t="s">
         <v>82</v>
       </c>
-      <c r="F13" s="61" t="s">
+      <c r="F13" s="62" t="s">
         <v>83</v>
       </c>
-      <c r="G13" s="62" t="n">
-        <v>1</v>
-      </c>
-      <c r="H13" s="63" t="n">
-        <v>1</v>
-      </c>
-      <c r="I13" s="62" t="n">
-        <v>1</v>
-      </c>
-      <c r="J13" s="63" t="n">
+      <c r="G13" s="63" t="n">
+        <v>1</v>
+      </c>
+      <c r="H13" s="64" t="n">
+        <v>1</v>
+      </c>
+      <c r="I13" s="63" t="n">
+        <v>1</v>
+      </c>
+      <c r="J13" s="64" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2817,140 +2821,140 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.3198380566802"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="40.5991902834008"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.4939271255061"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="38.0283400809717"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="24.5303643724696"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="25.2793522267206"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.5303643724696"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="41.2388663967611"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.7085020242915"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="38.668016194332"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="24.9595141700405"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="25.6032388663968"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1" s="37" t="s">
+      <c r="B1" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="37" t="s">
+      <c r="C1" s="38" t="s">
         <v>71</v>
       </c>
-      <c r="D1" s="37" t="s">
+      <c r="D1" s="38" t="s">
         <v>72</v>
       </c>
-      <c r="E1" s="37" t="s">
+      <c r="E1" s="38" t="s">
         <v>73</v>
       </c>
-      <c r="F1" s="37" t="s">
+      <c r="F1" s="38" t="s">
         <v>74</v>
       </c>
-      <c r="G1" s="37" t="s">
+      <c r="G1" s="38" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="40" t="s">
+      <c r="B2" s="41" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="41" t="s">
+      <c r="C2" s="42" t="s">
         <v>75</v>
       </c>
-      <c r="D2" s="42"/>
-      <c r="E2" s="41" t="s">
+      <c r="D2" s="43"/>
+      <c r="E2" s="42" t="s">
         <v>75</v>
       </c>
-      <c r="F2" s="44" t="n">
+      <c r="F2" s="45" t="n">
         <v>7613035220065</v>
       </c>
-      <c r="G2" s="46" t="s">
+      <c r="G2" s="47" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="47" t="s">
+      <c r="B3" s="48" t="s">
         <v>31</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="D3" s="48"/>
+      <c r="D3" s="49"/>
       <c r="E3" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="F3" s="50" t="n">
+      <c r="F3" s="51" t="n">
         <v>7613034954459</v>
       </c>
-      <c r="G3" s="52" t="s">
+      <c r="G3" s="53" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="47" t="s">
+      <c r="B4" s="48" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="53" t="s">
+      <c r="C4" s="54" t="s">
         <v>77</v>
       </c>
-      <c r="D4" s="54"/>
-      <c r="E4" s="53" t="s">
+      <c r="D4" s="55"/>
+      <c r="E4" s="54" t="s">
         <v>77</v>
       </c>
-      <c r="F4" s="56" t="n">
+      <c r="F4" s="57" t="n">
         <v>7613035058347</v>
       </c>
-      <c r="G4" s="52" t="s">
+      <c r="G4" s="53" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="47" t="s">
+      <c r="B5" s="48" t="s">
         <v>31</v>
       </c>
-      <c r="C5" s="53" t="s">
+      <c r="C5" s="54" t="s">
         <v>78</v>
       </c>
-      <c r="D5" s="54"/>
-      <c r="E5" s="53" t="s">
+      <c r="D5" s="55"/>
+      <c r="E5" s="54" t="s">
         <v>78</v>
       </c>
-      <c r="F5" s="56" t="n">
+      <c r="F5" s="57" t="n">
         <v>7613034872630</v>
       </c>
-      <c r="G5" s="52" t="s">
+      <c r="G5" s="53" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="47" t="s">
+      <c r="B6" s="48" t="s">
         <v>31</v>
       </c>
-      <c r="C6" s="53" t="s">
+      <c r="C6" s="54" t="s">
         <v>81</v>
       </c>
-      <c r="D6" s="54"/>
-      <c r="E6" s="53" t="s">
+      <c r="D6" s="55"/>
+      <c r="E6" s="54" t="s">
         <v>81</v>
       </c>
-      <c r="F6" s="56" t="n">
+      <c r="F6" s="57" t="n">
         <v>7613035738119</v>
       </c>
-      <c r="G6" s="52" t="s">
+      <c r="G6" s="53" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="30.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="64" t="s">
+      <c r="B7" s="65" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="58" t="s">
+      <c r="C7" s="59" t="s">
         <v>82</v>
       </c>
-      <c r="D7" s="65"/>
-      <c r="E7" s="60" t="s">
+      <c r="D7" s="66"/>
+      <c r="E7" s="61" t="s">
         <v>82</v>
       </c>
-      <c r="F7" s="60" t="s">
+      <c r="F7" s="61" t="s">
         <v>83</v>
       </c>
-      <c r="G7" s="63" t="s">
+      <c r="G7" s="64" t="s">
         <v>84</v>
       </c>
     </row>

</xml_diff>